<commit_message>
mise a jour RACI
commencement maquette reseau apres ca
</commit_message>
<xml_diff>
--- a/Documents/Matrice RACI Reseau/Matrice_RACI_General.xlsx
+++ b/Documents/Matrice RACI Reseau/Matrice_RACI_General.xlsx
@@ -152,10 +152,10 @@
     <t>Mise en place des matrices RACI</t>
   </si>
   <si>
-    <t>RIC</t>
-  </si>
-  <si>
     <t>Mettre en place la première infrastructure réseau sous packetracer ( maquette )</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -1180,7 +1180,7 @@
   <dimension ref="B1:I23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,7 +1335,7 @@
     </row>
     <row r="15" spans="2:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="51" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" s="32"/>
       <c r="D15" s="44" t="s">
@@ -1393,10 +1393,10 @@
         <v>34</v>
       </c>
       <c r="E18" s="49" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G18" s="7"/>
       <c r="H18" s="8"/>

</xml_diff>

<commit_message>
Avancement RACI Reseau et QRCODE liée BDD
A terminer de ma part , vous pouvez upload et push mais sans toucher au qrcode pour l'instant la famille, vous pouvez modificer la matrice RACI
</commit_message>
<xml_diff>
--- a/Documents/Matrice RACI Reseau/Matrice_RACI_General.xlsx
+++ b/Documents/Matrice RACI Reseau/Matrice_RACI_General.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azn_j\Desktop\ESGI\2017-2018\Projet_annuel\Projet_Annuel2i\Documents\Matrice RACI Reseau\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azn_j\Desktop\Projet_Annuel2i_save\Documents\Matrice RACI Reseau\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="58">
   <si>
     <t>RACI Chart (Roles and Responsibilities Matrix)</t>
   </si>
@@ -146,19 +146,64 @@
     <t>Creation et mise a jour du diagramme de Gantz</t>
   </si>
   <si>
-    <t>Mise a jour du document du projet ( nom, logo … ) et idées des premieres fonctionnalités</t>
-  </si>
-  <si>
-    <t>Mise en place des matrices RACI</t>
-  </si>
-  <si>
-    <t>Mettre en place la première infrastructure réseau sous packetracer ( maquette )</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
     <t>Application QRCODE</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Prestataire</t>
+  </si>
+  <si>
+    <t>RESEAU</t>
+  </si>
+  <si>
+    <t>APPLICATION C</t>
+  </si>
+  <si>
+    <t>DEVELOPPEMENT WEB</t>
+  </si>
+  <si>
+    <t>ANALYSE DU CACHIER DES CHARGES</t>
+  </si>
+  <si>
+    <t>Chiffrage financier</t>
+  </si>
+  <si>
+    <t>Analyse du Besoin</t>
+  </si>
+  <si>
+    <t>Mise a jour du cahier des charges</t>
+  </si>
+  <si>
+    <t>Application de sortie/entrée XML</t>
+  </si>
+  <si>
+    <t>Mise en place de la base de donnée</t>
+  </si>
+  <si>
+    <t>Charte graphiques du site web</t>
+  </si>
+  <si>
+    <t>creations des matrices RACI</t>
+  </si>
+  <si>
+    <t>MCD ET MLD</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Choix du template</t>
+  </si>
+  <si>
+    <t>Html / Css</t>
+  </si>
+  <si>
+    <t>Developpement Dynamique</t>
   </si>
 </sst>
 </file>
@@ -275,7 +320,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -300,8 +345,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -534,6 +585,58 @@
     </border>
     <border>
       <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -579,7 +682,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -596,12 +699,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -652,29 +749,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -799,6 +875,68 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1180,10 +1318,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:I23"/>
+  <dimension ref="B1:I35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1198,7 +1336,7 @@
   <sheetData>
     <row r="1" spans="2:9" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:9" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="32" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="2"/>
@@ -1207,7 +1345,7 @@
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="42"/>
+      <c r="B3" s="33"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -1225,27 +1363,27 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="2:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="29" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="53" t="s">
+      <c r="D5" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="55"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="46"/>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="58"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="49"/>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="2:9" ht="7.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1259,17 +1397,17 @@
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="29" t="s">
         <v>25</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="39">
+      <c r="D8" s="30">
         <v>43136</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="40">
+      <c r="F8" s="31">
         <v>43136</v>
       </c>
       <c r="G8" s="3"/>
@@ -1287,27 +1425,27 @@
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="2:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="29" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="59" t="s">
+      <c r="D10" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="61"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="52"/>
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="2:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="64"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="55"/>
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1320,156 +1458,440 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="14" spans="2:9" ht="25.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="43" t="s">
+    <row r="14" spans="2:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-    </row>
-    <row r="15" spans="2:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="51" t="s">
+      <c r="G14" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="44" t="s">
+      <c r="H14" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="76" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="77"/>
+      <c r="D15" s="78" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="78" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" s="30"/>
-      <c r="H15" s="31"/>
-    </row>
-    <row r="16" spans="2:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="52" t="s">
+      <c r="G15" s="78" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="78" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="28"/>
+      <c r="D16" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="45" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="G16" s="7"/>
-      <c r="H16" s="8"/>
-    </row>
-    <row r="17" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="51" t="s">
+      <c r="G16" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="86" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="28"/>
+      <c r="D17" s="84" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="89" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="89" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="86" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="28"/>
+      <c r="D18" s="84" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="89" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" s="89" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="86" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="90" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" s="86" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="46" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" s="48" t="s">
+      <c r="C20" s="28"/>
+      <c r="D20" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="F17" s="48" t="s">
-        <v>36</v>
-      </c>
-      <c r="G17" s="33"/>
-      <c r="H17" s="34"/>
-    </row>
-    <row r="18" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="52" t="s">
+      <c r="F20" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" s="86" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21" s="86" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="79" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="80"/>
+      <c r="D22" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="82" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" s="83" t="s">
+        <v>36</v>
+      </c>
+      <c r="G22" s="87" t="s">
+        <v>33</v>
+      </c>
+      <c r="H22" s="88" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="45" t="s">
+      <c r="C23" s="28"/>
+      <c r="D23" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="49" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G18" s="7"/>
-      <c r="H18" s="8"/>
-    </row>
-    <row r="19" spans="2:8" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="51" t="s">
+      <c r="E23" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="G23" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" s="86" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="28"/>
+      <c r="D24" s="74" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="75" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="75" t="s">
+        <v>33</v>
+      </c>
+      <c r="G24" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24" s="86" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="79" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="80"/>
+      <c r="D25" s="81" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="82" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" s="82" t="s">
+        <v>38</v>
+      </c>
+      <c r="G25" s="87" t="s">
+        <v>33</v>
+      </c>
+      <c r="H25" s="88" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="95" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="18"/>
+      <c r="D26" s="91" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="92" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" s="92" t="s">
+        <v>36</v>
+      </c>
+      <c r="G26" s="93" t="s">
+        <v>33</v>
+      </c>
+      <c r="H26" s="94" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="95" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="18"/>
+      <c r="D27" s="91" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="92" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" s="92" t="s">
+        <v>38</v>
+      </c>
+      <c r="G27" s="93" t="s">
+        <v>33</v>
+      </c>
+      <c r="H27" s="94" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="95" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="18"/>
+      <c r="D28" s="91" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="92" t="s">
+        <v>54</v>
+      </c>
+      <c r="F28" s="92" t="s">
+        <v>38</v>
+      </c>
+      <c r="G28" s="93" t="s">
+        <v>33</v>
+      </c>
+      <c r="H28" s="94" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="95" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="18"/>
+      <c r="D29" s="91" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="92" t="s">
+        <v>34</v>
+      </c>
+      <c r="F29" s="92" t="s">
+        <v>38</v>
+      </c>
+      <c r="G29" s="93" t="s">
+        <v>33</v>
+      </c>
+      <c r="H29" s="94" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="95" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="91" t="s">
+        <v>36</v>
+      </c>
+      <c r="E30" s="92" t="s">
+        <v>34</v>
+      </c>
+      <c r="F30" s="92" t="s">
+        <v>38</v>
+      </c>
+      <c r="G30" s="93" t="s">
+        <v>33</v>
+      </c>
+      <c r="H30" s="94" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="79" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="32"/>
-      <c r="D19" s="47" t="s">
+      <c r="C31" s="80"/>
+      <c r="D31" s="81" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="82" t="s">
+        <v>36</v>
+      </c>
+      <c r="F31" s="82" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="35"/>
-      <c r="H19" s="36"/>
-    </row>
-    <row r="20" spans="2:8" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="52" t="s">
+      <c r="G31" s="87" t="s">
+        <v>33</v>
+      </c>
+      <c r="H31" s="88" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="45" t="s">
+      <c r="C32" s="6"/>
+      <c r="D32" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E32" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="49" t="s">
+      <c r="F32" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="G20" s="9"/>
-      <c r="H20" s="8"/>
-    </row>
-    <row r="21" spans="2:8" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="51" t="s">
+      <c r="G32" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="H32" s="86" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="32"/>
-      <c r="D21" s="47" t="s">
+      <c r="C33" s="28"/>
+      <c r="D33" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="50" t="s">
+      <c r="E33" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="F21" s="50" t="s">
+      <c r="F33" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="G21" s="37"/>
-      <c r="H21" s="36"/>
-    </row>
-    <row r="22" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="65" t="s">
+      <c r="G33" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="H33" s="86" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D35" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="66"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="67"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="57"/>
+      <c r="G35" s="57"/>
+      <c r="H35" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="D5:H6"/>
     <mergeCell ref="D10:H11"/>
-    <mergeCell ref="D23:H23"/>
+    <mergeCell ref="D35:H35"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1488,235 +1910,235 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.69921875" style="11" customWidth="1"/>
-    <col min="2" max="2" width="38.796875" style="11" customWidth="1"/>
-    <col min="3" max="3" width="2.296875" style="11" customWidth="1"/>
-    <col min="4" max="8" width="15.796875" style="11" customWidth="1"/>
-    <col min="9" max="9" width="1.19921875" style="11" customWidth="1"/>
-    <col min="10" max="16384" width="10.796875" style="11"/>
+    <col min="1" max="1" width="1.69921875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="38.796875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="2.296875" style="9" customWidth="1"/>
+    <col min="4" max="8" width="15.796875" style="9" customWidth="1"/>
+    <col min="9" max="9" width="1.19921875" style="9" customWidth="1"/>
+    <col min="10" max="16384" width="10.796875" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:9" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
     </row>
     <row r="3" spans="2:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="2:9" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="14"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="12"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="71" t="s">
+      <c r="C5" s="12"/>
+      <c r="D5" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="14"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="12"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="76"/>
-      <c r="I6" s="14"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="12"/>
     </row>
     <row r="7" spans="2:9" ht="7.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="17" t="s">
+      <c r="C8" s="12"/>
+      <c r="D8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
     </row>
     <row r="9" spans="2:9" ht="7.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="16"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
     </row>
     <row r="10" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="77" t="s">
+      <c r="C10" s="12"/>
+      <c r="D10" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="78"/>
-      <c r="F10" s="78"/>
-      <c r="G10" s="78"/>
-      <c r="H10" s="79"/>
-      <c r="I10" s="14"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="12"/>
     </row>
     <row r="11" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="80"/>
-      <c r="E11" s="81"/>
-      <c r="F11" s="81"/>
-      <c r="G11" s="81"/>
-      <c r="H11" s="82"/>
-      <c r="I11" s="14"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="72"/>
+      <c r="H11" s="73"/>
+      <c r="I11" s="12"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
     </row>
     <row r="14" spans="2:9" ht="25.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="G14" s="18" t="s">
+      <c r="G14" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="23"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="21"/>
     </row>
     <row r="16" spans="2:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="26"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="24"/>
     </row>
     <row r="17" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="26"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="24"/>
     </row>
     <row r="18" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="26"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="24"/>
     </row>
     <row r="19" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="26"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="24"/>
     </row>
     <row r="20" spans="2:8" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="29"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="27"/>
     </row>
     <row r="21" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="68" t="s">
+      <c r="D22" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="69"/>
-      <c r="F22" s="69"/>
-      <c r="G22" s="69"/>
-      <c r="H22" s="70"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="61"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H24" s="11" t="s">
+      <c r="H24" s="9" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>